<commit_message>
Modificando o Kanban e criando novas atividades no mesmo
</commit_message>
<xml_diff>
--- a/Artefatos de Documentação/Processo Aplicado/EveRemind/2-Gerencia de Projeto/Kanban - EveRemind.xlsx
+++ b/Artefatos de Documentação/Processo Aplicado/EveRemind/2-Gerencia de Projeto/Kanban - EveRemind.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moises\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leonardo\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>Kanban EveRemind</t>
   </si>
@@ -85,6 +85,24 @@
   </si>
   <si>
     <t>Fazer</t>
+  </si>
+  <si>
+    <t>Criar Servlet para manter categoria e criar atividade</t>
+  </si>
+  <si>
+    <t>Criar interface para criação para manter categoria, criar atividade e confirmar email</t>
+  </si>
+  <si>
+    <t>Criar interface para manter atividade e ver a atividade</t>
+  </si>
+  <si>
+    <t>Criar Servlet para manter atividade</t>
+  </si>
+  <si>
+    <t>Criar comunicação com o banco de dados para manter a atividade.</t>
+  </si>
+  <si>
+    <t>Criar conexão com o banco para Servlets e classe que envia email de autenticação</t>
   </si>
 </sst>
 </file>
@@ -162,7 +180,7 @@
       <name val="Aral"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -178,12 +196,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -237,7 +249,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -264,6 +276,9 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -271,9 +286,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -283,10 +298,58 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -297,64 +360,19 @@
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Título" xfId="1" builtinId="15"/>
+    <cellStyle name="Title" xfId="1" builtinId="15"/>
   </cellStyles>
   <dxfs count="9">
     <dxf>
@@ -557,9 +575,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -597,7 +615,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -669,7 +687,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -821,17 +839,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13:D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="90.42578125" customWidth="1"/>
-    <col min="3" max="3" width="74.140625" customWidth="1"/>
-    <col min="4" max="4" width="78.28515625" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="76.42578125" customWidth="1"/>
+    <col min="3" max="3" width="90.85546875" customWidth="1"/>
+    <col min="4" max="4" width="91" customWidth="1"/>
+    <col min="5" max="5" width="4.42578125" customWidth="1"/>
     <col min="6" max="6" width="44" customWidth="1"/>
   </cols>
   <sheetData>
@@ -875,164 +893,177 @@
       <c r="A4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="12" t="s">
+      <c r="B4" s="35"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
     </row>
     <row r="5" spans="1:6" ht="35.1" customHeight="1">
       <c r="A5" s="9"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="16" t="s">
+      <c r="B5" s="11"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="13"/>
-      <c r="F5" s="17" t="s">
+      <c r="E5" s="10"/>
+      <c r="F5" s="14" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="35.1" customHeight="1">
       <c r="A6" s="9"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="20" t="s">
+      <c r="B6" s="15"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="21"/>
-      <c r="F6" s="22" t="s">
+      <c r="E6" s="18"/>
+      <c r="F6" s="19" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="35.1" customHeight="1">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="12" t="s">
+      <c r="B7" s="35"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="24" t="s">
+      <c r="E7" s="18"/>
+      <c r="F7" s="21" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="35.1" customHeight="1">
-      <c r="A8" s="23"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="25" t="s">
+      <c r="A8" s="20"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="15"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="26" t="s">
+      <c r="E8" s="18"/>
+      <c r="F8" s="23" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="35.1" customHeight="1">
-      <c r="A9" s="23"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="20" t="s">
+      <c r="A9" s="20"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="19"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="13"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="10"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="27"/>
-      <c r="B10" s="28"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="13"/>
+      <c r="A10" s="24"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="10"/>
     </row>
     <row r="11" spans="1:6" ht="35.1" customHeight="1">
-      <c r="A11" s="27"/>
-      <c r="B11" s="30" t="s">
+      <c r="A11" s="24"/>
+      <c r="B11" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="29"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="13"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="10"/>
     </row>
     <row r="12" spans="1:6" ht="35.1" customHeight="1">
-      <c r="A12" s="31" t="s">
+      <c r="A12" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="33" t="s">
+      <c r="C12" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="33" t="s">
+      <c r="D12" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="21"/>
-      <c r="F12" s="13"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="10"/>
     </row>
     <row r="13" spans="1:6" ht="35.1" customHeight="1">
-      <c r="A13" s="34" t="s">
+      <c r="A13" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="35"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="13"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="39"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="10"/>
     </row>
     <row r="14" spans="1:6" ht="35.1" customHeight="1">
-      <c r="A14" s="29"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="13"/>
+      <c r="A14" s="26"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="13"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="10"/>
     </row>
     <row r="15" spans="1:6" ht="35.1" customHeight="1">
-      <c r="A15" s="36"/>
-      <c r="B15" s="37"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="13"/>
+      <c r="A15" s="32"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="40"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="10"/>
     </row>
     <row r="16" spans="1:6" ht="35.1" customHeight="1">
-      <c r="A16" s="36" t="s">
+      <c r="A16" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="13"/>
+      <c r="B16" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="10"/>
     </row>
     <row r="17" spans="1:6" ht="35.1" customHeight="1">
-      <c r="A17" s="38"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="13"/>
+      <c r="A17" s="34"/>
+      <c r="B17" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="10"/>
     </row>
     <row r="18" spans="1:6" ht="35.1" customHeight="1">
-      <c r="A18" s="36"/>
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="13"/>
+      <c r="A18" s="32"/>
+      <c r="B18" s="40" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[GPR] Atualizando as atividades no Kanban e adicionando o Sprint 3
</commit_message>
<xml_diff>
--- a/Artefatos de Documentação/Processo Aplicado/EveRemind/2-Gerencia de Projeto/Kanban - EveRemind.xlsx
+++ b/Artefatos de Documentação/Processo Aplicado/EveRemind/2-Gerencia de Projeto/Kanban - EveRemind.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leonardo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leonardo\Dropbox\Repositórios\GitHub\P.I.-ES-UFG-2015-BIJLMMV\Artefatos de Documentação\Processo Aplicado\EveRemind\2-Gerencia de Projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="33">
   <si>
     <t>Kanban EveRemind</t>
   </si>
@@ -103,6 +103,27 @@
   </si>
   <si>
     <t>Criar conexão com o banco para Servlets e classe que envia email de autenticação</t>
+  </si>
+  <si>
+    <t>Sprint 3</t>
+  </si>
+  <si>
+    <t>Criar interface para visualizar atividades em lista</t>
+  </si>
+  <si>
+    <t>Criar o Servlet para pegar as atividades em lista</t>
+  </si>
+  <si>
+    <t>Criar a conexão com o banco para pegar todas as atividades</t>
+  </si>
+  <si>
+    <t>Criar interface para visualizar atividades em calendario</t>
+  </si>
+  <si>
+    <t>Criar o Servlet para pegar as atividades em forma cronológica</t>
+  </si>
+  <si>
+    <t>Criar comunicação com o bd para pegar atividades cronologicamente</t>
   </si>
 </sst>
 </file>
@@ -180,7 +201,7 @@
       <name val="Aral"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -225,18 +246,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -244,12 +259,90 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -339,18 +432,9 @@
     <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -367,6 +451,81 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -837,10 +996,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13:D15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -893,9 +1052,9 @@
       <c r="A4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="35"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="37" t="s">
+      <c r="B4" s="32"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="34" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="10"/>
@@ -929,9 +1088,9 @@
       <c r="A7" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="35"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37" t="s">
+      <c r="B7" s="32"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34" t="s">
         <v>13</v>
       </c>
       <c r="E7" s="18"/>
@@ -969,7 +1128,7 @@
       <c r="E10" s="18"/>
       <c r="F10" s="10"/>
     </row>
-    <row r="11" spans="1:6" ht="35.1" customHeight="1">
+    <row r="11" spans="1:6" ht="34.5" customHeight="1">
       <c r="A11" s="24"/>
       <c r="B11" s="27" t="s">
         <v>18</v>
@@ -995,69 +1154,143 @@
       <c r="E12" s="18"/>
       <c r="F12" s="10"/>
     </row>
-    <row r="13" spans="1:6" ht="35.1" customHeight="1">
-      <c r="A13" s="31" t="s">
+    <row r="13" spans="1:6" ht="34.5" customHeight="1">
+      <c r="A13" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="38"/>
-      <c r="C13" s="39" t="s">
+      <c r="B13" s="35"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="39"/>
       <c r="E13" s="18"/>
       <c r="F13" s="10"/>
     </row>
     <row r="14" spans="1:6" ht="35.1" customHeight="1">
       <c r="A14" s="26"/>
       <c r="B14" s="12"/>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="13"/>
+      <c r="D14" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="13"/>
       <c r="E14" s="18"/>
       <c r="F14" s="10"/>
     </row>
     <row r="15" spans="1:6" ht="35.1" customHeight="1">
-      <c r="A15" s="32"/>
-      <c r="B15" s="33"/>
-      <c r="C15" s="40" t="s">
+      <c r="A15" s="26"/>
+      <c r="B15" s="31"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="40"/>
       <c r="E15" s="18"/>
       <c r="F15" s="10"/>
     </row>
     <row r="16" spans="1:6" ht="35.1" customHeight="1">
-      <c r="A16" s="32" t="s">
+      <c r="A16" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="39" t="s">
+      <c r="B16" s="36"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
       <c r="E16" s="18"/>
       <c r="F16" s="10"/>
     </row>
     <row r="17" spans="1:6" ht="35.1" customHeight="1">
-      <c r="A17" s="34"/>
-      <c r="B17" s="13" t="s">
+      <c r="A17" s="60"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
       <c r="E17" s="18"/>
       <c r="F17" s="10"/>
     </row>
     <row r="18" spans="1:6" ht="35.1" customHeight="1">
-      <c r="A18" s="32"/>
-      <c r="B18" s="40" t="s">
+      <c r="A18" s="60"/>
+      <c r="B18" s="37"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="40"/>
-      <c r="D18" s="40"/>
       <c r="E18" s="18"/>
       <c r="F18" s="10"/>
+    </row>
+    <row r="20" spans="1:6" ht="33.75" customHeight="1">
+      <c r="A20" s="38"/>
+      <c r="B20" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="43"/>
+      <c r="D20" s="44"/>
+    </row>
+    <row r="21" spans="1:6" ht="33.75" customHeight="1">
+      <c r="A21" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" s="46" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="47" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="48" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="33.75" customHeight="1">
+      <c r="A22" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="40"/>
+      <c r="C22" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="49"/>
+    </row>
+    <row r="23" spans="1:6" ht="33.75" customHeight="1">
+      <c r="A23" s="50"/>
+      <c r="B23" s="51"/>
+      <c r="C23" s="51" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="52"/>
+    </row>
+    <row r="24" spans="1:6" ht="33.75" customHeight="1">
+      <c r="A24" s="59"/>
+      <c r="B24" s="41"/>
+      <c r="C24" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="D24" s="53"/>
+    </row>
+    <row r="25" spans="1:6" ht="33.75" customHeight="1">
+      <c r="A25" s="61" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="54" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" s="54"/>
+      <c r="D25" s="55"/>
+    </row>
+    <row r="26" spans="1:6" ht="33.75" customHeight="1">
+      <c r="A26" s="62"/>
+      <c r="B26" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" s="56"/>
+      <c r="D26" s="39"/>
+    </row>
+    <row r="27" spans="1:6" ht="33.75" customHeight="1">
+      <c r="A27" s="61"/>
+      <c r="B27" s="57" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" s="57"/>
+      <c r="D27" s="58"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
[GPR] Atualização do status do sprint 3 no Kanban
</commit_message>
<xml_diff>
--- a/Artefatos de Documentação/Processo Aplicado/EveRemind/2-Gerencia de Projeto/Kanban - EveRemind.xlsx
+++ b/Artefatos de Documentação/Processo Aplicado/EveRemind/2-Gerencia de Projeto/Kanban - EveRemind.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leonardo\Dropbox\Repositórios\GitHub\P.I.-ES-UFG-2015-BIJLMMV\Artefatos de Documentação\Processo Aplicado\EveRemind\2-Gerencia de Projeto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moises\Dropbox\UFG\5º Período\Projeto Integrador\P.I.-ES-UFG-2015-BIJLMMV\Artefatos de Documentação\Processo Aplicado\EveRemind\2-Gerencia de Projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -342,7 +342,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -486,19 +486,10 @@
     <xf numFmtId="0" fontId="12" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -531,7 +522,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Title" xfId="1" builtinId="15"/>
+    <cellStyle name="Título" xfId="1" builtinId="15"/>
   </cellStyles>
   <dxfs count="9">
     <dxf>
@@ -734,9 +725,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -774,7 +765,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -846,7 +837,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -998,8 +989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1187,7 +1178,7 @@
       <c r="F15" s="10"/>
     </row>
     <row r="16" spans="1:6" ht="35.1" customHeight="1">
-      <c r="A16" s="60" t="s">
+      <c r="A16" s="57" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="36"/>
@@ -1199,7 +1190,7 @@
       <c r="F16" s="10"/>
     </row>
     <row r="17" spans="1:6" ht="35.1" customHeight="1">
-      <c r="A17" s="60"/>
+      <c r="A17" s="57"/>
       <c r="B17" s="13"/>
       <c r="C17" s="13"/>
       <c r="D17" s="13" t="s">
@@ -1209,7 +1200,7 @@
       <c r="F17" s="10"/>
     </row>
     <row r="18" spans="1:6" ht="35.1" customHeight="1">
-      <c r="A18" s="60"/>
+      <c r="A18" s="57"/>
       <c r="B18" s="37"/>
       <c r="C18" s="37"/>
       <c r="D18" s="37" t="s">
@@ -1245,52 +1236,52 @@
         <v>6</v>
       </c>
       <c r="B22" s="40"/>
-      <c r="C22" s="40" t="s">
+      <c r="C22" s="40"/>
+      <c r="D22" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="D22" s="49"/>
     </row>
     <row r="23" spans="1:6" ht="33.75" customHeight="1">
-      <c r="A23" s="50"/>
-      <c r="B23" s="51"/>
-      <c r="C23" s="51" t="s">
+      <c r="A23" s="49"/>
+      <c r="B23" s="50"/>
+      <c r="C23" s="50"/>
+      <c r="D23" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="52"/>
     </row>
     <row r="24" spans="1:6" ht="33.75" customHeight="1">
-      <c r="A24" s="59"/>
+      <c r="A24" s="56"/>
       <c r="B24" s="41"/>
-      <c r="C24" s="41" t="s">
+      <c r="C24" s="41"/>
+      <c r="D24" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="D24" s="53"/>
     </row>
     <row r="25" spans="1:6" ht="33.75" customHeight="1">
-      <c r="A25" s="61" t="s">
+      <c r="A25" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="54" t="s">
+      <c r="B25" s="51"/>
+      <c r="C25" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="54"/>
-      <c r="D25" s="55"/>
+      <c r="D25" s="52"/>
     </row>
     <row r="26" spans="1:6" ht="33.75" customHeight="1">
-      <c r="A26" s="62"/>
-      <c r="B26" s="56" t="s">
+      <c r="A26" s="59"/>
+      <c r="B26" s="53"/>
+      <c r="C26" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="C26" s="56"/>
       <c r="D26" s="39"/>
     </row>
     <row r="27" spans="1:6" ht="33.75" customHeight="1">
-      <c r="A27" s="61"/>
-      <c r="B27" s="57" t="s">
+      <c r="A27" s="58"/>
+      <c r="B27" s="54"/>
+      <c r="C27" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="C27" s="57"/>
-      <c r="D27" s="58"/>
+      <c r="D27" s="55"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>